<commit_message>
Water level historical values and norm data support changes
</commit_message>
<xml_diff>
--- a/sapphire_backend/static/templates/discharge_norm_decadal_template.xlsx
+++ b/sapphire_backend/static/templates/discharge_norm_decadal_template.xlsx
@@ -5,10 +5,11 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="discharge" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="discharge" sheetId="1" state="visible" r:id="rId3"/>
+    <sheet name="water_level" sheetId="2" state="visible" r:id="rId4"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -20,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="38">
   <si>
     <t xml:space="preserve">Period</t>
   </si>
@@ -228,11 +229,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -248,8 +249,256 @@
 </styleSheet>
 </file>
 
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Office">
+  <a:themeElements>
+    <a:clrScheme name="LibreOffice">
+      <a:dk1>
+        <a:srgbClr val="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:srgbClr val="ffffff"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="000000"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="ffffff"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="18a303"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="0369a3"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="a33e03"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="8e03a3"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="c99c00"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="c9211e"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0000ee"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="551a8b"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Arial" pitchFamily="0" charset="1"/>
+        <a:ea typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+        <a:cs typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Arial" pitchFamily="0" charset="1"/>
+        <a:ea typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+        <a:cs typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme>
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:prstDash val="solid"/>
+          <a:miter/>
+        </a:ln>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:prstDash val="solid"/>
+          <a:miter/>
+        </a:ln>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:prstDash val="solid"/>
+          <a:miter/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+</a:theme>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:AK2"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetData>
+    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="U1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="V1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="W1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="X1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="Y1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="Z1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="AA1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="AB1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="AC1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="AD1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="AE1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="AF1" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="AG1" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="AH1" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="AI1" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="AJ1" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="AK1" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
@@ -261,7 +510,7 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
-    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>

</xml_diff>